<commit_message>
update CYRS review sheet
</commit_message>
<xml_diff>
--- a/Input Documents/CYRS/CYRS_Review.xlsx
+++ b/Input Documents/CYRS/CYRS_Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -190,11 +190,14 @@
 Customer Req : xx           : xx 
 if the version of the refernce document is not exist or status keep this fields empty </t>
   </si>
+  <si>
+    <t xml:space="preserve">Update the status </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -494,7 +497,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -562,12 +565,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,34 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -946,7 +952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -956,200 +962,225 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-    </row>
-    <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25" t="s">
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="31">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="25">
+        <v>1.3</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
-    </row>
-    <row r="9" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
-    </row>
-    <row r="10" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="41">
+        <v>44014</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="32"/>
-    </row>
-    <row r="14" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="41">
+        <v>44014</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1166,23 +1197,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1193,24 +1207,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -1239,7 +1253,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>30</v>
       </c>
@@ -1262,11 +1276,11 @@
         <v>21</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>30</v>
       </c>
@@ -1289,14 +1303,14 @@
         <v>21</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I3" s="10"/>
       <c r="K3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
@@ -1319,14 +1333,14 @@
         <v>21</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I4" s="10"/>
       <c r="K4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
@@ -1349,11 +1363,11 @@
         <v>21</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1376,14 +1390,14 @@
         <v>21</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I6" s="12"/>
       <c r="K6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1406,14 +1420,14 @@
         <v>21</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I7" s="12"/>
       <c r="K7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>30</v>
       </c>
@@ -1436,11 +1450,11 @@
         <v>21</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
@@ -1467,7 +1481,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1484,7 +1498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1501,7 +1515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1512,7 +1526,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1523,7 +1537,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1534,7 +1548,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1545,7 +1559,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1556,7 +1570,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1567,7 +1581,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1578,7 +1592,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1589,7 +1603,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1600,7 +1614,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1611,7 +1625,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1622,7 +1636,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1633,7 +1647,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1644,7 +1658,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1655,7 +1669,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1666,7 +1680,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1677,7 +1691,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1688,7 +1702,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1699,7 +1713,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1710,7 +1724,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1721,7 +1735,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1732,7 +1746,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1743,7 +1757,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1754,7 +1768,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1765,7 +1779,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1776,7 +1790,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1787,7 +1801,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1798,7 +1812,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1809,7 +1823,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1820,7 +1834,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1831,7 +1845,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1842,7 +1856,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1853,7 +1867,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1864,7 +1878,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1875,7 +1889,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>

</xml_diff>